<commit_message>
schema update and sample schema json added
</commit_message>
<xml_diff>
--- a/Source/_meta_scripts/_docs/R2-DataSchema.xlsx
+++ b/Source/_meta_scripts/_docs/R2-DataSchema.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etkvh/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DC073F-6C06-BF49-9DE6-304005C93167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="756" windowWidth="30240" windowHeight="17976"/>
   </bookViews>
   <sheets>
     <sheet name="R2-Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,35 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={876E17C0-B755-4CD8-A897-29554D9C81F6}</author>
-  </authors>
-  <commentList>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{876E17C0-B755-4CD8-A897-29554D9C81F6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Either Add VirtualCare and PassLinkCloud as product Type or keep this field as optional</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
-  <si>
-    <t>*mark in green means newly added</t>
-  </si>
-  <si>
-    <t>*mark in red means obsoleted</t>
-  </si>
-  <si>
-    <t>This is for Passlink Device user manage like PLC, PLM, TWX-US, TWS-EU (mandatory field validation would be based on UserSystemType)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="105">
   <si>
     <t>PL-Device-Users</t>
   </si>
@@ -140,9 +108,6 @@
     <t>UserProductInjectorIDs</t>
   </si>
   <si>
-    <t>could be 501# or TPA# or SRUid-Serial#</t>
-  </si>
-  <si>
     <t>UserTokenExpiryTime</t>
   </si>
   <si>
@@ -224,51 +189,9 @@
     <t>iPhone, iPad, AndroidPhone, Tablet, Other</t>
   </si>
   <si>
-    <t>UserIsPassLinkServiceAccess</t>
-  </si>
-  <si>
-    <t>Boolean Flag; default value as true</t>
-  </si>
-  <si>
-    <t>default = true</t>
-  </si>
-  <si>
-    <t>UserIsSWBundleAccess</t>
-  </si>
-  <si>
-    <t>Boolean Flag;  default value as true</t>
-  </si>
-  <si>
-    <t>UserIsMandatoryTypeSWBundleAccess</t>
-  </si>
-  <si>
-    <t>UserIsEntitlementTypeSWBundleAccess</t>
-  </si>
-  <si>
-    <t>UserIsSoftwareInstallAccess</t>
-  </si>
-  <si>
-    <t>UserIsGrabInjectorSWStatusAccess</t>
-  </si>
-  <si>
-    <t>UserIsRemoteSWBundleInstallAccess</t>
-  </si>
-  <si>
-    <t>Boolean Flag;  default value as false</t>
-  </si>
-  <si>
-    <t>for remote unlock by QR to do SWInstall</t>
-  </si>
-  <si>
     <t>UserSourceSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">EnumList Values {PLM, PLC, TWX-US, TWS-EU}  </t>
-  </si>
-  <si>
-    <t>default = mobile; TW is also an user for interacting with CLOUD APIs</t>
-  </si>
-  <si>
     <t>UserOrganizationName</t>
   </si>
   <si>
@@ -383,14 +306,53 @@
     <t xml:space="preserve">Default value = '' (for BIOMED only) </t>
   </si>
   <si>
-    <t>GLOBAL, USERManagement, LogOnly</t>
+    <t>UserCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnumList Values {PLM, PLC}  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">default = mobile; </t>
+  </si>
+  <si>
+    <t>GLOBAL, UserManagementOnly, LogOnly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could be 501# or TPA# or SRUid-Serial# ["ProductType-Serial#"]  </t>
+  </si>
+  <si>
+    <t>This is for Passlink Device user manage like PLC, PLM as UserSystemType</t>
+  </si>
+  <si>
+    <t>configId</t>
+  </si>
+  <si>
+    <t>keyName</t>
+  </si>
+  <si>
+    <t>keyValue</t>
+  </si>
+  <si>
+    <t>Unique Id</t>
+  </si>
+  <si>
+    <t>Name of Config</t>
+  </si>
+  <si>
+    <t>Value of Config</t>
+  </si>
+  <si>
+    <t>*if any mark in green means newly added</t>
+  </si>
+  <si>
+    <t>*if any mark in red means obsoleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,12 +471,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Karthikeyan Ranganathan" id="{DBB86D7B-BCEA-47D0-9FD1-7C15D34CFFAD}" userId="S::karthikeyan.ranganathan@bayer.com::15763092-969f-4ee7-9c8a-e1a6e459609b" providerId="AD"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -558,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -610,7 +566,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -804,759 +760,663 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C12" dT="2024-01-10T14:16:33.67" personId="{DBB86D7B-BCEA-47D0-9FD1-7C15D34CFFAD}" id="{876E17C0-B755-4CD8-A897-29554D9C81F6}">
-    <text>Either Add VirtualCare and PassLinkCloud as product Type or keep this field as optional</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="58.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="109.5" customWidth="1"/>
-    <col min="6" max="6" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="64.6640625" customWidth="1"/>
+    <col min="6" max="6" width="70.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1">
+      <c r="A3" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="13.8">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:6">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="1:6">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="4" t="s">
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="4" t="s">
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:7">
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:7">
       <c r="C19" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7">
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" s="9" customFormat="1">
+      <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13.8" customHeight="1">
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
-        <v>51</v>
-      </c>
+    <row r="25" spans="2:7">
       <c r="C25" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="4"/>
+    <row r="26" spans="2:7">
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F26" s="4"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7">
       <c r="C27" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" s="9" customFormat="1">
       <c r="C28" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" s="9" customFormat="1">
       <c r="C29" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7">
       <c r="C30" s="4" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:7">
       <c r="C31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" ht="13.8">
+      <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="4" t="s">
+      <c r="C35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="C36" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="4" t="s">
+      <c r="D36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="4" t="s">
+    </row>
+    <row r="37" spans="1:7">
+      <c r="C37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="2:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="C34" s="4" t="s">
+      <c r="D37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="5" t="s">
+    </row>
+    <row r="38" spans="1:7">
+      <c r="C38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="4" t="s">
+      <c r="D38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="F38" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="C39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="D39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="4" t="s">
+      <c r="F39" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="9" customFormat="1">
+      <c r="C40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="D40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="4" t="s">
+    </row>
+    <row r="41" spans="1:7">
+      <c r="C41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="4" t="s">
+      <c r="D41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="F41" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="4" t="s">
+      <c r="D42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="2:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B41" s="2" t="s">
+      <c r="F42" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="C43" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="4" t="s">
+      <c r="D43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="F43" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="C44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="D44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="4" t="s">
+      <c r="F44" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:7">
       <c r="C47" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="13.8">
       <c r="C48" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" s="4" customFormat="1" ht="13.8">
       <c r="C49" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C50" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="50" spans="3:5" s="4" customFormat="1" ht="13.8"/>
+    <row r="51" spans="3:5" s="4" customFormat="1" ht="13.8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;22&amp;KFF8939 RESTRICTED</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f10c8667-ffa8-410b-9edd-4cada14a77af" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063A8FE9D32DB5D438E3A6F020D52B174" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6847b9a3f58562cd0dee443fc3ea0196">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce" xmlns:ns3="f10c8667-ffa8-410b-9edd-4cada14a77af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c0e46f7f713e10bbfb0b44c64ad89a4" ns2:_="" ns3:_="">
     <xsd:import namespace="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce"/>
@@ -1805,10 +1665,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f10c8667-ffa8-410b-9edd-4cada14a77af" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59717EB1-149F-48B5-8F7C-1B775FE01821}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C19E429-9758-42CA-B7BB-4E4B9AF1356C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce"/>
+    <ds:schemaRef ds:uri="f10c8667-ffa8-410b-9edd-4cada14a77af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1825,20 +1716,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C19E429-9758-42CA-B7BB-4E4B9AF1356C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59717EB1-149F-48B5-8F7C-1B775FE01821}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a7dc6fb1-b0ce-4cb4-bb30-4c65e261d8ce"/>
-    <ds:schemaRef ds:uri="f10c8667-ffa8-410b-9edd-4cada14a77af"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>